<commit_message>
add hybrid parameter passing feature
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ct_FeatureBranch\US4835_ChangeVariableDeclaration\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ct_FeatureBranch\US493143_HybridParameterPassing\codeless_test\target\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13176" windowHeight="6408" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13176" windowHeight="6408" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
   <si>
     <t>key</t>
   </si>
@@ -140,9 +140,6 @@
     <t>sendKeys</t>
   </si>
   <si>
-    <t>seattle</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
     <t>https://www.bing.com/</t>
   </si>
   <si>
-    <t>{{searchBar}}</t>
-  </si>
-  <si>
     <t>searchBar</t>
   </si>
   <si>
@@ -303,6 +297,12 @@
   </si>
   <si>
     <t>bing.yahoopage.searchbutton</t>
+  </si>
+  <si>
+    <t>{{empId}}</t>
+  </si>
+  <si>
+    <t>assertEquals::WebDriver::getTitle::{{empId}}</t>
   </si>
 </sst>
 </file>
@@ -821,101 +821,101 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="C13" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C15" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="C16" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="C17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="15"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>33</v>
@@ -931,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -941,7 +941,7 @@
     <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="75.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
@@ -983,96 +983,96 @@
     </row>
     <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="F3" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -1080,26 +1080,29 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>37</v>
+        <v>90</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>86</v>
@@ -1108,10 +1111,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1139,7 +1142,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>35</v>
@@ -1147,23 +1150,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1171,10 +1174,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1189,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1201,42 +1204,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made new data sheets and new models
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ct_FeatureBranch\US4835_ChangeVariableDeclaration\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\repos\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA752B2-4FA3-4869-9E13-63BD318EA389}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13176" windowHeight="6408" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13180" windowHeight="6410" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
     <sheet name="t-googletest" sheetId="9" r:id="rId2"/>
-    <sheet name="d-dataSheet" sheetId="10" r:id="rId3"/>
-    <sheet name="d-dev" sheetId="11" r:id="rId4"/>
+    <sheet name="t-mapstest" sheetId="12" r:id="rId3"/>
+    <sheet name="t-tmotest" sheetId="13" r:id="rId4"/>
+    <sheet name="d-dataSheet" sheetId="10" r:id="rId5"/>
+    <sheet name="d-dev" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>key</t>
   </si>
@@ -140,9 +143,6 @@
     <t>sendKeys</t>
   </si>
   <si>
-    <t>seattle</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -303,12 +303,69 @@
   </si>
   <si>
     <t>bing.yahoopage.searchbutton</t>
+  </si>
+  <si>
+    <t>bothell</t>
+  </si>
+  <si>
+    <t>Google.googlepage.searchbutton2</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps</t>
+  </si>
+  <si>
+    <t>maps.mapspage.searchbox</t>
+  </si>
+  <si>
+    <t>enter address</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>tmobile headquarters</t>
+  </si>
+  <si>
+    <t>query search</t>
+  </si>
+  <si>
+    <t>maps.mapspage.searchbutton</t>
+  </si>
+  <si>
+    <t>{{address}}</t>
+  </si>
+  <si>
+    <t>tmopage</t>
+  </si>
+  <si>
+    <t>https://www.tmobile.com</t>
+  </si>
+  <si>
+    <t>{{tmopage}}</t>
+  </si>
+  <si>
+    <t>navigate to tmobile page</t>
+  </si>
+  <si>
+    <t>navigate to google maps</t>
+  </si>
+  <si>
+    <t>click menu</t>
+  </si>
+  <si>
+    <t>tmo.tmopage.menu</t>
+  </si>
+  <si>
+    <t>tmo.tmopage.joinlink</t>
+  </si>
+  <si>
+    <t>click Join us option</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -705,22 +762,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6328125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="7"/>
+    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.6328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -731,7 +788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -742,7 +799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
@@ -753,7 +810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -764,7 +821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -775,7 +832,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
@@ -786,7 +843,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -797,7 +854,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
@@ -808,7 +865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
@@ -819,103 +876,103 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="9" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="9" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+      <c r="B12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="11" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="B17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>33</v>
@@ -928,27 +985,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -970,7 +1027,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -981,140 +1038,140 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="F3" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>66</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
     </row>
   </sheetData>
@@ -1124,124 +1181,326 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEB8117-E754-4E19-8B29-956FB96AE5DB}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.36328125" customWidth="1"/>
+    <col min="2" max="2" width="35.08984375" customWidth="1"/>
+    <col min="3" max="3" width="32.90625" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>88</v>
+      <c r="B6" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{84775297-0440-4095-927B-0BC25FD41393}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B942603-42C6-4993-9A8D-64F68066BDF1}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="42.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{ECF5FD2F-CC08-4F76-B2E9-46133F3E3160}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Bugfix/fix u itestsreadingfromlib models"
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -2,22 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\CTA\github\codeless\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ct_FeatureBranch\US493143_HybridParameterPassing\codeless_test\target\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13185" windowHeight="6405" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13176" windowHeight="6408" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
     <sheet name="t-googletest" sheetId="9" r:id="rId2"/>
-    <sheet name="t-mapstest" sheetId="12" r:id="rId3"/>
-    <sheet name="t-tmotest" sheetId="13" r:id="rId4"/>
-    <sheet name="d-dataSheet" sheetId="10" r:id="rId5"/>
-    <sheet name="d-dev" sheetId="11" r:id="rId6"/>
+    <sheet name="d-dataSheet" sheetId="10" r:id="rId3"/>
+    <sheet name="d-dev" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
   <si>
     <t>key</t>
   </si>
@@ -299,60 +297,6 @@
   </si>
   <si>
     <t>bing.yahoopage.searchbutton</t>
-  </si>
-  <si>
-    <t>Google.googlepage.searchbutton2</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps</t>
-  </si>
-  <si>
-    <t>maps.mapspage.searchbox</t>
-  </si>
-  <si>
-    <t>enter address</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>tmobile headquarters</t>
-  </si>
-  <si>
-    <t>query search</t>
-  </si>
-  <si>
-    <t>maps.mapspage.searchbutton</t>
-  </si>
-  <si>
-    <t>{{address}}</t>
-  </si>
-  <si>
-    <t>tmopage</t>
-  </si>
-  <si>
-    <t>https://www.tmobile.com</t>
-  </si>
-  <si>
-    <t>{{tmopage}}</t>
-  </si>
-  <si>
-    <t>navigate to tmobile page</t>
-  </si>
-  <si>
-    <t>navigate to google maps</t>
-  </si>
-  <si>
-    <t>click menu</t>
-  </si>
-  <si>
-    <t>tmo.tmopage.menu</t>
-  </si>
-  <si>
-    <t>tmo.tmopage.joinlink</t>
-  </si>
-  <si>
-    <t>click Join us option</t>
   </si>
   <si>
     <t>{{empId}}</t>
@@ -364,7 +308,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -764,19 +708,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.42578125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.5703125" style="7"/>
+    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -787,7 +731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -798,7 +742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
@@ -809,7 +753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -820,7 +764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -831,7 +775,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
@@ -842,7 +786,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -853,7 +797,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
@@ -864,7 +808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
@@ -875,7 +819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
@@ -886,7 +830,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>41</v>
       </c>
@@ -897,7 +841,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>44</v>
       </c>
@@ -908,7 +852,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>45</v>
       </c>
@@ -919,7 +863,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
@@ -930,7 +874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>48</v>
       </c>
@@ -941,7 +885,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>50</v>
       </c>
@@ -952,7 +896,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>52</v>
       </c>
@@ -963,13 +907,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>55</v>
       </c>
@@ -987,24 +931,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="75.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1026,19 +970,18 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="12"/>
+      <c r="D2" s="3"/>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>76</v>
       </c>
@@ -1059,7 +1002,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>77</v>
       </c>
@@ -1078,7 +1021,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>74</v>
       </c>
@@ -1099,7 +1042,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>75</v>
       </c>
@@ -1120,7 +1063,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>78</v>
       </c>
@@ -1135,7 +1078,7 @@
       <c r="F7" s="13"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>79</v>
       </c>
@@ -1146,15 +1089,15 @@
         <v>83</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>87</v>
       </c>
@@ -1165,21 +1108,16 @@
         <v>86</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>81</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
     </row>
   </sheetData>
@@ -1190,97 +1128,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1288,185 +1190,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1474,7 +1210,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>64</v>
       </c>
@@ -1482,7 +1218,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>72</v>
       </c>
@@ -1490,7 +1226,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>80</v>
       </c>
@@ -1498,7 +1234,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
add new sampletest with omdb
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ct_FeatureBranch\US493143_HybridParameterPassing\codeless_test\target\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CE5BA8-B579-415D-A21A-EC0D8F1A7F01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13176" windowHeight="6408" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13180" windowHeight="6410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
     <sheet name="t-googletest" sheetId="9" r:id="rId2"/>
-    <sheet name="d-dataSheet" sheetId="10" r:id="rId3"/>
-    <sheet name="d-dev" sheetId="11" r:id="rId4"/>
+    <sheet name="t-omdb&amp;imdb" sheetId="12" r:id="rId3"/>
+    <sheet name="d-dataSheet" sheetId="10" r:id="rId4"/>
+    <sheet name="d-dev" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="122">
   <si>
     <t>key</t>
   </si>
@@ -203,112 +205,202 @@
     <t>POST</t>
   </si>
   <si>
-    <t>body::string::{"name":"etp","salary":"123456789","age":"100"}</t>
-  </si>
-  <si>
     <t>customer.api.v1.employee.{id}</t>
   </si>
   <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>dummy.restapiexample.com</t>
+  </si>
+  <si>
+    <t>apiHost</t>
+  </si>
+  <si>
+    <t>goto</t>
+  </si>
+  <si>
+    <t>{{website}}</t>
+  </si>
+  <si>
+    <t>/api/v1/create</t>
+  </si>
+  <si>
+    <t>apiPath</t>
+  </si>
+  <si>
+    <t>sample.api.create</t>
+  </si>
+  <si>
+    <t>searchElement</t>
+  </si>
+  <si>
+    <t>close browser</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>{{searchElement}}</t>
+  </si>
+  <si>
+    <t>https://www.bing.com/</t>
+  </si>
+  <si>
+    <t>searchBar</t>
+  </si>
+  <si>
+    <t>Google.googlepage.searchbutton</t>
+  </si>
+  <si>
+    <t>bing.yahoopage.searchbar</t>
+  </si>
+  <si>
+    <t>bing.yahoopage.searchbutton</t>
+  </si>
+  <si>
+    <t>omdbhost</t>
+  </si>
+  <si>
+    <t>http://www.omdbapi.com</t>
+  </si>
+  <si>
+    <t>omdbpath</t>
+  </si>
+  <si>
+    <t>endpoint::host::{{omdbhost}}::path::{{omdbpath}}</t>
+  </si>
+  <si>
+    <t>export::wall-e_plot::JSONPATH::Plot</t>
+  </si>
+  <si>
+    <t>imdb</t>
+  </si>
+  <si>
+    <t>?apikey=91999f16&amp;i=tt0910970</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>customer.api.v1.delete.{id}</t>
+  </si>
+  <si>
+    <t>assertEquals::WebElement::getText::{{wall-e_plot}}</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt1049413/</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0910970/</t>
+  </si>
+  <si>
+    <t>imdb2</t>
+  </si>
+  <si>
+    <t>{{imdb2}}</t>
+  </si>
+  <si>
+    <t>waitType::waitForPageLoad</t>
+  </si>
+  <si>
+    <t>waitTime::6000</t>
+  </si>
+  <si>
+    <t>imdb.imdbpage.searchbar</t>
+  </si>
+  <si>
+    <t>wall-e</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com</t>
+  </si>
+  <si>
+    <t>waitType::visible</t>
+  </si>
+  <si>
+    <t>imdbhome</t>
+  </si>
+  <si>
+    <t>{{imdbhome}}</t>
+  </si>
+  <si>
+    <t>imdb.imdbpage.wall-e</t>
+  </si>
+  <si>
+    <t>waitType::clickable</t>
+  </si>
+  <si>
+    <t>imdb.imdbpage.submit</t>
+  </si>
+  <si>
+    <t>imdb.imdbpage.plot</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>Navigate to UI page</t>
+  </si>
+  <si>
+    <t>assertNotEquals::WebElement::getText::{{wall-e_plot}}</t>
+  </si>
+  <si>
+    <t>#navigate to imdb for up</t>
+  </si>
+  <si>
+    <t>omdb call</t>
+  </si>
+  <si>
+    <t>home page</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>click search button</t>
+  </si>
+  <si>
+    <t>click on wall-e result</t>
+  </si>
+  <si>
+    <t>wait for wall-e page to load</t>
+  </si>
+  <si>
+    <t>t-mobile best network</t>
+  </si>
+  <si>
+    <t>path::id::{{empId}}</t>
+  </si>
+  <si>
     <t>export::empId::JSONPATH::id</t>
   </si>
   <si>
-    <t>path::id::{{empId}}</t>
-  </si>
-  <si>
-    <t>website</t>
-  </si>
-  <si>
-    <t>dummy.restapiexample.com</t>
-  </si>
-  <si>
-    <t>apiHost</t>
-  </si>
-  <si>
-    <t>endpoint::host::dummy.restapiexample.com::protocol::http::path::/api/v1/create</t>
-  </si>
-  <si>
-    <t>goto</t>
-  </si>
-  <si>
-    <t>{{website}}</t>
-  </si>
-  <si>
-    <t>bodytemplate::namevar::codeless::salaryvar::100::agevar::20</t>
-  </si>
-  <si>
-    <t>bodytemplate::namevar::etpcodeless::salaryvar::400::agevar::23</t>
-  </si>
-  <si>
-    <t>endpoint::host::{{apiHost}}::path::{{apiPath}}</t>
-  </si>
-  <si>
-    <t>/api/v1/create</t>
-  </si>
-  <si>
-    <t>apiPath</t>
-  </si>
-  <si>
-    <t>sample.api.create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overide dynamically on sample api's body and endpoint </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overide on sample api's body and endpoint </t>
+    <t>export::empsalary::JSONPATH::salary</t>
+  </si>
+  <si>
+    <t>{{empsalary}}</t>
+  </si>
+  <si>
+    <t>GET call from customer api</t>
   </si>
   <si>
     <t>POST call to customer api</t>
   </si>
   <si>
-    <t>GET call from customer api</t>
-  </si>
-  <si>
-    <t>Navigate to UI page</t>
-  </si>
-  <si>
-    <t>Search on UI page</t>
-  </si>
-  <si>
-    <t>searchElement</t>
-  </si>
-  <si>
-    <t>close browser</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>{{searchElement}}</t>
-  </si>
-  <si>
-    <t>https://www.bing.com/</t>
-  </si>
-  <si>
-    <t>searchBar</t>
-  </si>
-  <si>
-    <t>Google.googlepage.searchbutton</t>
-  </si>
-  <si>
-    <t>#button</t>
-  </si>
-  <si>
-    <t>bing.yahoopage.searchbar</t>
-  </si>
-  <si>
-    <t>bing.yahoopage.searchbutton</t>
-  </si>
-  <si>
-    <t>{{empId}}</t>
-  </si>
-  <si>
-    <t>assertEquals::WebDriver::getTitle::{{empId}}</t>
+    <t>type salary of employee created</t>
+  </si>
+  <si>
+    <t>body::string::{"name":"etptest","salary":"123456789","age":"100"}</t>
+  </si>
+  <si>
+    <t>delete call from customer api</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -705,22 +797,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6328125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="7"/>
+    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.6328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -731,7 +823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -742,7 +834,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
@@ -753,7 +845,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -764,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -775,7 +867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
@@ -786,7 +878,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -797,7 +889,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
@@ -808,7 +900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
@@ -819,7 +911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
@@ -830,7 +922,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>41</v>
       </c>
@@ -841,7 +933,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>44</v>
       </c>
@@ -852,7 +944,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>45</v>
       </c>
@@ -863,7 +955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
@@ -874,7 +966,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>48</v>
       </c>
@@ -885,7 +977,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>50</v>
       </c>
@@ -896,7 +988,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>52</v>
       </c>
@@ -907,13 +999,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>55</v>
       </c>
@@ -928,27 +1020,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="75.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.08984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -967,10 +1059,12 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -981,9 +1075,9 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>25</v>
@@ -995,130 +1089,112 @@
         <v>57</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="13" t="s">
+      <c r="B9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1127,124 +1203,386 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5F6690-B5F2-4AD4-892B-F827304863FC}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="33.90625" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" customWidth="1"/>
+    <col min="5" max="5" width="57.36328125" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="13"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{5EF3C7A3-CF75-47EA-BBC2-BFD51143ADB8}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{C01CCE07-37BB-4478-ADA7-B3EBC5233ECB}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{BB55764C-F14E-4ECB-ADA8-FE888D5590CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add "Description" column to SampleTest.xlsx spreadsheet in case you need a better explanation of the step than the step name Add "description" property and *ALL* the associated updates to the java entities and proceses to support it.
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO8\codeless_mastertestdata\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mposlus1\Documents\GitHub\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAEA645-45C2-4C9D-A616-E78787BA38F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
   <si>
     <t>key</t>
   </si>
@@ -289,94 +290,118 @@
     <t>type salary of employee created</t>
   </si>
   <si>
+    <t>delete call from customer api</t>
+  </si>
+  <si>
+    <t>webdriver.parentTunnel</t>
+  </si>
+  <si>
+    <t>webdriver.tunnelIdentifier</t>
+  </si>
+  <si>
+    <t>waitTime</t>
+  </si>
+  <si>
+    <t>webdriver.e34:token</t>
+  </si>
+  <si>
+    <t>webdriver.e34:video</t>
+  </si>
+  <si>
+    <t>webdriver.e34:l_testName</t>
+  </si>
+  <si>
+    <t>webdriver.e34:per_test_timeout_ms</t>
+  </si>
+  <si>
+    <t>type title of the page</t>
+  </si>
+  <si>
+    <t>{{title}}</t>
+  </si>
+  <si>
+    <t>export::title::WebDriver::getTitle</t>
+  </si>
+  <si>
+    <t>{{empId}}</t>
+  </si>
+  <si>
+    <t>7000</t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
+    <t>export::abc::WebElement::getText</t>
+  </si>
+  <si>
+    <t>get text of the element</t>
+  </si>
+  <si>
+    <t>move to the search bar</t>
+  </si>
+  <si>
+    <t>{{abc}}</t>
+  </si>
+  <si>
+    <t>get call to customer api</t>
+  </si>
+  <si>
+    <t>path::id::{{abc}}</t>
+  </si>
+  <si>
+    <t>assertEquals::WebDriver::getTitle::{{title}}</t>
+  </si>
+  <si>
+    <t>{{element1}}</t>
+  </si>
+  <si>
+    <t>{{txtBox}}</t>
+  </si>
+  <si>
+    <t>{{btnClick}}</t>
+  </si>
+  <si>
+    <t>testdata.filename</t>
+  </si>
+  <si>
+    <t>testdata.sheetname</t>
+  </si>
+  <si>
+    <t>testdata.xlsx</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>This is where we load the configuration information</t>
+  </si>
+  <si>
     <t>body::string::{"name":"etptest","salary":"123456789","age":"100"}</t>
   </si>
   <si>
-    <t>delete call from customer api</t>
-  </si>
-  <si>
-    <t>webdriver.parentTunnel</t>
-  </si>
-  <si>
-    <t>webdriver.tunnelIdentifier</t>
-  </si>
-  <si>
-    <t>waitTime</t>
-  </si>
-  <si>
-    <t>webdriver.e34:token</t>
-  </si>
-  <si>
-    <t>webdriver.e34:video</t>
-  </si>
-  <si>
-    <t>webdriver.e34:l_testName</t>
-  </si>
-  <si>
-    <t>webdriver.e34:per_test_timeout_ms</t>
-  </si>
-  <si>
-    <t>type title of the page</t>
-  </si>
-  <si>
-    <t>{{title}}</t>
-  </si>
-  <si>
-    <t>export::title::WebDriver::getTitle</t>
-  </si>
-  <si>
-    <t>{{empId}}</t>
-  </si>
-  <si>
-    <t>7000</t>
-  </si>
-  <si>
-    <t>move</t>
-  </si>
-  <si>
-    <t>export::abc::WebElement::getText</t>
-  </si>
-  <si>
-    <t>get text of the element</t>
-  </si>
-  <si>
-    <t>move to the search bar</t>
-  </si>
-  <si>
-    <t>{{abc}}</t>
-  </si>
-  <si>
-    <t>get call to customer api</t>
-  </si>
-  <si>
-    <t>path::id::{{abc}}</t>
-  </si>
-  <si>
-    <t>assertEquals::WebDriver::getTitle::{{title}}</t>
-  </si>
-  <si>
-    <t>{{element1}}</t>
-  </si>
-  <si>
-    <t>{{txtBox}}</t>
-  </si>
-  <si>
-    <t>{{btnClick}}</t>
-  </si>
-  <si>
-    <t>testdata.filename</t>
-  </si>
-  <si>
-    <t>testdata.sheetname</t>
-  </si>
-  <si>
-    <t>testdata.xlsx</t>
+    <t>Making a POST call to create some data</t>
+  </si>
+  <si>
+    <t>Making a GET call to confirm the creation</t>
+  </si>
+  <si>
+    <t>Deleting the data we created</t>
+  </si>
+  <si>
+    <t>Navigating to whatever website we identified</t>
+  </si>
+  <si>
+    <t>Clicking the Search button</t>
+  </si>
+  <si>
+    <t>Closing the browser because we're done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,22 +797,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="7"/>
+    <col min="1" max="1" width="36.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -798,7 +823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -809,7 +834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -820,7 +845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -831,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
@@ -842,7 +867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -853,7 +878,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -864,7 +889,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -875,7 +900,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>35</v>
       </c>
@@ -886,7 +911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>36</v>
       </c>
@@ -897,7 +922,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>38</v>
       </c>
@@ -908,7 +933,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -919,7 +944,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>41</v>
       </c>
@@ -930,7 +955,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
@@ -941,49 +966,49 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>90</v>
-      </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="15"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>46</v>
       </c>
@@ -991,25 +1016,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1019,27 +1044,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.77734375" style="1"/>
+    <col min="9" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1061,9 +1086,11 @@
       <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H1" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1073,8 +1100,11 @@
       <c r="D2" s="3"/>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>85</v>
       </c>
@@ -1088,7 +1118,7 @@
         <v>48</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>83</v>
@@ -1096,8 +1126,11 @@
       <c r="G3" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>84</v>
       </c>
@@ -1115,10 +1148,13 @@
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>18</v>
@@ -1134,8 +1170,11 @@
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>72</v>
       </c>
@@ -1147,8 +1186,11 @@
         <v>51</v>
       </c>
       <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>86</v>
       </c>
@@ -1156,36 +1198,36 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>78</v>
       </c>
@@ -1193,49 +1235,52 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
         <v>68</v>
       </c>
       <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
         <v>65</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>18</v>
@@ -1247,10 +1292,10 @@
         <v>25</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>53</v>
       </c>
@@ -1259,8 +1304,11 @@
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
   </sheetData>
@@ -1270,25 +1318,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1312,7 +1360,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1324,7 +1372,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>75</v>
       </c>
@@ -1345,7 +1393,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>76</v>
       </c>
@@ -1364,7 +1412,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>77</v>
       </c>
@@ -1385,7 +1433,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>78</v>
       </c>
@@ -1404,7 +1452,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
@@ -1423,7 +1471,7 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>80</v>
       </c>
@@ -1444,7 +1492,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>74</v>
       </c>
@@ -1467,7 +1515,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Added new field in config for uiactionlog
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mposlus1\Documents\GitHub\codeless\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO9\codeless_ui_action_log\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAEA645-45C2-4C9D-A616-E78787BA38F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
   <si>
     <t>key</t>
   </si>
@@ -396,13 +395,22 @@
   </si>
   <si>
     <t>Closing the browser because we're done</t>
+  </si>
+  <si>
+    <t>uiActionLog.details.enabled</t>
+  </si>
+  <si>
+    <t>codeless.plugins</t>
+  </si>
+  <si>
+    <t>com.tmobile.etp.codeless.plugin.reporting.CodelessPluginManager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +468,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -488,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -515,6 +529,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -797,22 +814,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.42578125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="7"/>
+    <col min="1" max="1" width="36.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -823,7 +840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -834,7 +851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -845,7 +862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -856,7 +873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
@@ -867,7 +884,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -878,7 +895,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -889,7 +906,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -900,7 +917,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>35</v>
       </c>
@@ -911,7 +928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>36</v>
       </c>
@@ -922,7 +939,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>38</v>
       </c>
@@ -933,7 +950,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -944,7 +961,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>41</v>
       </c>
@@ -955,7 +972,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
@@ -966,75 +983,91 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>94</v>
       </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B24" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="11" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1044,27 +1077,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1090,7 +1123,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1104,7 +1137,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>85</v>
       </c>
@@ -1130,7 +1163,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>84</v>
       </c>
@@ -1152,7 +1185,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>87</v>
       </c>
@@ -1174,7 +1207,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>72</v>
       </c>
@@ -1190,7 +1223,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>86</v>
       </c>
@@ -1209,7 +1242,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>95</v>
       </c>
@@ -1227,7 +1260,7 @@
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>78</v>
       </c>
@@ -1246,7 +1279,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>102</v>
       </c>
@@ -1264,7 +1297,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>103</v>
       </c>
@@ -1278,7 +1311,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>105</v>
       </c>
@@ -1295,7 +1328,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>53</v>
       </c>
@@ -1308,7 +1341,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
     </row>
   </sheetData>
@@ -1318,25 +1351,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="57.28515625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1393,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1372,7 +1405,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>75</v>
       </c>
@@ -1393,7 +1426,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>76</v>
       </c>
@@ -1412,7 +1445,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>77</v>
       </c>
@@ -1433,7 +1466,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>78</v>
       </c>
@@ -1452,7 +1485,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
@@ -1471,7 +1504,7 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>80</v>
       </c>
@@ -1492,7 +1525,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>74</v>
       </c>
@@ -1515,7 +1548,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Changed to 7 in config.properties and resolved the conflicts
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="128">
   <si>
     <t>key</t>
   </si>
@@ -325,9 +325,6 @@
     <t>{{empId}}</t>
   </si>
   <si>
-    <t>7000</t>
-  </si>
-  <si>
     <t>move</t>
   </si>
   <si>
@@ -370,40 +367,49 @@
     <t>testdata.xlsx</t>
   </si>
   <si>
+    <t>codeless.plugins</t>
+  </si>
+  <si>
+    <t>com.tmobile.etp.codeless.plugin.reporting.CodelessPluginManager</t>
+  </si>
+  <si>
+    <t>body::string::{"name":"etptest-100","salary":"123456789","age":"100"}</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>This is where we load the configuration information</t>
-  </si>
-  <si>
-    <t>body::string::{"name":"etptest","salary":"123456789","age":"100"}</t>
-  </si>
-  <si>
-    <t>Making a POST call to create some data</t>
-  </si>
-  <si>
-    <t>Making a GET call to confirm the creation</t>
-  </si>
-  <si>
-    <t>Deleting the data we created</t>
-  </si>
-  <si>
-    <t>Navigating to whatever website we identified</t>
-  </si>
-  <si>
-    <t>Clicking the Search button</t>
-  </si>
-  <si>
-    <t>Closing the browser because we're done</t>
+    <t>Close the browser instance</t>
+  </si>
+  <si>
+    <t>Post some data to an api</t>
+  </si>
+  <si>
+    <t>Get that data to see if it was created</t>
+  </si>
+  <si>
+    <t>Delete that data as we don't need it now</t>
+  </si>
+  <si>
+    <t>Navigate to a website</t>
+  </si>
+  <si>
+    <t>Submit some salary information</t>
+  </si>
+  <si>
+    <t>Type the webpage name</t>
+  </si>
+  <si>
+    <t>make a call  to the api to validate the submitted salary information</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Wait time delay is seconds, not milliseconds</t>
   </si>
   <si>
     <t>uiActionLog.details.enabled</t>
-  </si>
-  <si>
-    <t>codeless.plugins</t>
-  </si>
-  <si>
-    <t>com.tmobile.etp.codeless.plugin.reporting.CodelessPluginManager</t>
   </si>
 </sst>
 </file>
@@ -817,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -995,45 +1001,45 @@
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>94</v>
       </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>46</v>
       </c>
@@ -1041,33 +1047,36 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>90</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="11" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
-        <v>124</v>
-      </c>
       <c r="B27" s="11" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1081,7 +1090,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1120,7 +1129,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1133,9 +1142,6 @@
       <c r="D2" s="3"/>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="1" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -1151,7 +1157,7 @@
         <v>48</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>83</v>
@@ -1160,7 +1166,7 @@
         <v>82</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -1182,7 +1188,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -1204,7 +1210,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -1220,7 +1226,7 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -1231,7 +1237,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>98</v>
@@ -1241,6 +1247,9 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -1250,15 +1259,18 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>96</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G8" s="5"/>
+      <c r="H8" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -1268,52 +1280,49 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
         <v>68</v>
       </c>
       <c r="F9" s="13"/>
-      <c r="H9" s="1" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
         <v>65</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>18</v>
@@ -1325,7 +1334,10 @@
         <v>25</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1338,7 +1350,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="H13" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1355,7 +1367,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1367,6 +1379,7 @@
     <col min="5" max="5" width="57.33203125" customWidth="1"/>
     <col min="6" max="6" width="35.44140625" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -1391,7 +1404,9 @@
       <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -1444,6 +1459,9 @@
         <v>62</v>
       </c>
       <c r="G4" s="5"/>
+      <c r="H4" s="12" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -1465,6 +1483,9 @@
         <v>62</v>
       </c>
       <c r="G5" s="5"/>
+      <c r="H5" s="12" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
@@ -1484,6 +1505,9 @@
         <v>62</v>
       </c>
       <c r="G6" s="5"/>
+      <c r="H6" s="12" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -1503,6 +1527,9 @@
         <v>62</v>
       </c>
       <c r="G7" s="5"/>
+      <c r="H7" s="12" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -1524,6 +1551,9 @@
       <c r="G8" s="12" t="s">
         <v>62</v>
       </c>
+      <c r="H8" s="12" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
@@ -1546,6 +1576,9 @@
       </c>
       <c r="G9" s="12" t="s">
         <v>62</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Re-update the spreasheet with "seconds" value vice "milliseconds" value
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mposlus1\Documents\GitHub\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7B37B8-5B22-4232-A3CF-614C451F7059}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE56C01-E9D5-4007-A41F-29901DE1B39F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>waitType::waitForPageLoad</t>
   </si>
   <si>
-    <t>waitTime::6000</t>
-  </si>
-  <si>
     <t>imdb.imdbpage.searchbar</t>
   </si>
   <si>
@@ -408,6 +405,9 @@
   </si>
   <si>
     <t>Wait time delay is seconds, not milliseconds</t>
+  </si>
+  <si>
+    <t>waitTime::6</t>
   </si>
 </sst>
 </file>
@@ -986,37 +986,37 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="15"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="15"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="15"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="15"/>
     </row>
@@ -1030,34 +1030,34 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1110,7 +1110,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
     </row>
     <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
@@ -1138,21 +1138,21 @@
         <v>48</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>18</v>
@@ -1164,17 +1164,17 @@
         <v>25</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>18</v>
@@ -1186,17 +1186,17 @@
         <v>57</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>50</v>
@@ -1207,103 +1207,103 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>18</v>
@@ -1315,10 +1315,10 @@
         <v>25</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1331,7 +1331,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="H13" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1386,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1403,7 +1403,7 @@
     </row>
     <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
@@ -1424,103 +1424,103 @@
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="12" t="s">
@@ -1530,36 +1530,36 @@
         <v>61</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>60</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>61</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added feature to allow all ui and service steps to take in dynamic and static values in same cell
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO9\codeless_etr_er_screenshots\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D0A529-1128-47E0-BD5D-1023EBCDC921}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -334,9 +335,6 @@
     <t>move to the search bar</t>
   </si>
   <si>
-    <t>{{abc}}</t>
-  </si>
-  <si>
     <t>get call to customer api</t>
   </si>
   <si>
@@ -428,12 +426,15 @@
   </si>
   <si>
     <t>assertNotEquals::WebDriver::getTitle::{{title}}</t>
+  </si>
+  <si>
+    <t>{{abc}} othervariable: {{othervar}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -838,22 +839,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="7"/>
+    <col min="1" max="1" width="36.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.6328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -864,7 +865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -875,7 +876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -886,7 +887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -897,7 +898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
@@ -908,7 +909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -919,7 +920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -930,7 +931,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -941,7 +942,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>35</v>
       </c>
@@ -952,7 +953,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>36</v>
       </c>
@@ -963,7 +964,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>38</v>
       </c>
@@ -974,7 +975,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -985,7 +986,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>41</v>
       </c>
@@ -996,7 +997,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
@@ -1007,60 +1008,60 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>90</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>92</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>46</v>
       </c>
@@ -1068,53 +1069,53 @@
         <v>26</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>89</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="11" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1124,27 +1125,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.6640625" style="1"/>
+    <col min="9" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1167,10 +1168,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1181,7 +1182,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>84</v>
       </c>
@@ -1195,7 +1196,7 @@
         <v>48</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>82</v>
@@ -1204,10 +1205,10 @@
         <v>81</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>83</v>
       </c>
@@ -1226,10 +1227,10 @@
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>86</v>
       </c>
@@ -1248,10 +1249,10 @@
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>71</v>
       </c>
@@ -1264,10 +1265,10 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>85</v>
       </c>
@@ -1275,7 +1276,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>97</v>
@@ -1286,10 +1287,10 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>94</v>
       </c>
@@ -1297,20 +1298,20 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>95</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>77</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
@@ -1326,7 +1327,7 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>100</v>
       </c>
@@ -1334,7 +1335,7 @@
         <v>98</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
@@ -1344,7 +1345,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>101</v>
       </c>
@@ -1352,15 +1353,15 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>18</v>
@@ -1372,13 +1373,13 @@
         <v>25</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>53</v>
       </c>
@@ -1388,10 +1389,10 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="H13" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
     </row>
   </sheetData>
@@ -1401,26 +1402,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.6328125" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="33.6328125" customWidth="1"/>
+    <col min="4" max="4" width="37.08984375" customWidth="1"/>
+    <col min="5" max="5" width="57.36328125" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1443,10 +1444,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1458,7 +1459,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>74</v>
       </c>
@@ -1479,7 +1480,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>75</v>
       </c>
@@ -1494,14 +1495,14 @@
         <v>61</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>76</v>
       </c>
@@ -1518,14 +1519,14 @@
         <v>64</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>77</v>
       </c>
@@ -1540,14 +1541,14 @@
         <v>67</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>78</v>
       </c>
@@ -1562,14 +1563,14 @@
         <v>67</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>79</v>
       </c>
@@ -1587,13 +1588,13 @@
         <v>61</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>73</v>
       </c>
@@ -1613,13 +1614,13 @@
         <v>61</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
updated sampletest to call postman request by name
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64005106-EB11-4B30-A3A6-A292D11E8CC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A13733C-EC82-41FC-9A89-B976234C5B85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>{{website}}</t>
   </si>
   <si>
-    <t>sample.api.create</t>
-  </si>
-  <si>
     <t>close browser</t>
   </si>
   <si>
@@ -423,6 +420,9 @@
   </si>
   <si>
     <t>assertEquals::WebDriver::getTitle::{{title}}</t>
+  </si>
+  <si>
+    <t>sample.dummyAPIs-POST</t>
   </si>
 </sst>
 </file>
@@ -930,7 +930,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>33</v>
@@ -1010,49 +1010,49 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="15"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" s="15"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" s="15"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
@@ -1063,53 +1063,53 @@
         <v>26</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1122,7 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1162,7 +1162,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1178,7 +1178,7 @@
     </row>
     <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
@@ -1190,21 +1190,21 @@
         <v>47</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>18</v>
@@ -1216,39 +1216,39 @@
         <v>25</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>49</v>
@@ -1259,103 +1259,103 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>18</v>
@@ -1367,23 +1367,23 @@
         <v>25</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>53</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="H13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1399,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1438,7 +1438,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1455,145 +1455,145 @@
     </row>
     <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="G8" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
         <v>52</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added configurations for sampletest
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO10\codeless_parallel_execution_2\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64005106-EB11-4B30-A3A6-A292D11E8CC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="137">
   <si>
     <t>key</t>
   </si>
@@ -347,12 +346,6 @@
     <t>testdata.xlsx</t>
   </si>
   <si>
-    <t>codeless.plugins</t>
-  </si>
-  <si>
-    <t>com.tmobile.etp.codeless.plugin.reporting.CodelessPluginManager</t>
-  </si>
-  <si>
     <t>body::string::{"name":"etptest-100","salary":"123456789","age":"100"}</t>
   </si>
   <si>
@@ -389,9 +382,6 @@
     <t>Wait time delay is seconds, not milliseconds</t>
   </si>
   <si>
-    <t>uiActionLog.details.enabled</t>
-  </si>
-  <si>
     <t>waitTime::6</t>
   </si>
   <si>
@@ -410,9 +400,6 @@
     <t>TRUE or FALSE</t>
   </si>
   <si>
-    <t>FAILUREONLY</t>
-  </si>
-  <si>
     <t>{{abc}} othervariable: {{othervar}}</t>
   </si>
   <si>
@@ -423,12 +410,39 @@
   </si>
   <si>
     <t>assertEquals::WebDriver::getTitle::{{title}}</t>
+  </si>
+  <si>
+    <t>test.runparallel</t>
+  </si>
+  <si>
+    <t>test.runparallel.threadcount</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>ALLSTEPS</t>
+  </si>
+  <si>
+    <t>uiactionlog.details.enabled</t>
+  </si>
+  <si>
+    <t>qTestTestRunId::85</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>To run in parallel set it to true (TRUE or FALSE)</t>
+  </si>
+  <si>
+    <t>Thread count config for parallel running</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -833,22 +847,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.6328125" style="7"/>
+    <col min="1" max="1" width="36.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -859,7 +873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -870,7 +884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -881,7 +895,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -892,7 +906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
@@ -903,7 +917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -914,7 +928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -925,18 +939,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -947,7 +961,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>35</v>
       </c>
@@ -958,7 +972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
@@ -969,7 +983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>38</v>
       </c>
@@ -980,7 +994,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
@@ -991,7 +1005,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>42</v>
       </c>
@@ -1002,114 +1016,128 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>83</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>86</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>88</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>89</v>
       </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B22" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
-      <c r="A23" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
-      <c r="A24" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+      <c r="A26" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
+      <c r="B27" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+      <c r="A28" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="11" t="s">
+      <c r="C28" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1119,27 +1147,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.6328125" style="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1162,10 +1190,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1173,10 +1201,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="3"/>
+      <c r="E2" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>80</v>
       </c>
@@ -1190,7 +1221,7 @@
         <v>47</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>78</v>
@@ -1199,10 +1230,10 @@
         <v>77</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>79</v>
       </c>
@@ -1221,10 +1252,10 @@
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>82</v>
       </c>
@@ -1243,10 +1274,10 @@
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>69</v>
       </c>
@@ -1259,10 +1290,10 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>81</v>
       </c>
@@ -1281,10 +1312,10 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>90</v>
       </c>
@@ -1298,14 +1329,14 @@
         <v>91</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>73</v>
       </c>
@@ -1321,7 +1352,7 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>96</v>
       </c>
@@ -1339,7 +1370,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>97</v>
       </c>
@@ -1350,10 +1381,10 @@
         <v>101</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>98</v>
       </c>
@@ -1370,10 +1401,10 @@
         <v>99</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>52</v>
       </c>
@@ -1383,10 +1414,10 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="H13" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
     </row>
   </sheetData>
@@ -1396,26 +1427,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.6328125" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="33.6328125" customWidth="1"/>
-    <col min="4" max="4" width="37.08984375" customWidth="1"/>
-    <col min="5" max="5" width="57.36328125" customWidth="1"/>
-    <col min="6" max="6" width="35.453125" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1438,10 +1469,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1453,7 +1484,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>70</v>
       </c>
@@ -1474,7 +1505,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>71</v>
       </c>
@@ -1489,14 +1520,14 @@
         <v>59</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>72</v>
       </c>
@@ -1513,14 +1544,14 @@
         <v>62</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>73</v>
       </c>
@@ -1535,14 +1566,14 @@
         <v>65</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>74</v>
       </c>
@@ -1557,14 +1588,14 @@
         <v>65</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>75</v>
       </c>
@@ -1582,13 +1613,13 @@
         <v>59</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
omdb/postman_collection.json: Update postman collection so that one of the items has a period in the name. sampletest.xlsx: Update the test that calls the above modified item request. PostmanParser.java:  Change item.folderName setter to use a period (.) instead of a slash (/) ServiceStepBuilder.java:  Update operation path builder to build a Postman operation path using periods instead of slashes.
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mposlus1\Documents\GitHub\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E510E3-2B33-45A0-A093-1BD9C76D18A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC95A75-B3CA-48D5-B3A8-6781609F1EEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26385" yWindow="2205" windowWidth="24600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="146">
   <si>
     <t>key</t>
   </si>
@@ -434,7 +434,37 @@
     <t>omdb call3</t>
   </si>
   <si>
-    <t>omdb.othermovies.scarymovies.Shaun of the Dead</t>
+    <t>true</t>
+  </si>
+  <si>
+    <t>test.runparallel</t>
+  </si>
+  <si>
+    <t>test.runparallel.threadcount</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>buildMode</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>qTestProjectId</t>
+  </si>
+  <si>
+    <t>qTestBuildMode</t>
+  </si>
+  <si>
+    <t>qTestTestRunId::85</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>omdb.othermovies.scarymovies.Shaun.of the Dead</t>
   </si>
 </sst>
 </file>
@@ -846,21 +876,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.6328125" style="7"/>
+    <col min="1" max="1" width="36.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -871,7 +901,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -882,7 +912,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -893,7 +923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -904,7 +934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
@@ -915,7 +945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -926,7 +956,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -937,7 +967,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -948,7 +978,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -959,7 +989,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>35</v>
       </c>
@@ -970,7 +1000,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
@@ -981,7 +1011,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>38</v>
       </c>
@@ -992,7 +1022,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
@@ -1003,7 +1033,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>42</v>
       </c>
@@ -1014,49 +1044,49 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>86</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>115</v>
       </c>
@@ -1067,7 +1097,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>45</v>
       </c>
@@ -1078,7 +1108,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>117</v>
       </c>
@@ -1089,7 +1119,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>83</v>
       </c>
@@ -1100,7 +1130,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>99</v>
       </c>
@@ -1111,17 +1141,57 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>102</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1138,20 +1208,20 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.6328125" style="1"/>
+    <col min="9" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1177,7 +1247,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1188,7 +1258,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>78</v>
       </c>
@@ -1214,7 +1284,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>77</v>
       </c>
@@ -1236,7 +1306,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>80</v>
       </c>
@@ -1258,7 +1328,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>67</v>
       </c>
@@ -1274,7 +1344,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
@@ -1296,7 +1366,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>88</v>
       </c>
@@ -1317,7 +1387,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
@@ -1333,7 +1403,7 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>94</v>
       </c>
@@ -1351,7 +1421,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>95</v>
       </c>
@@ -1365,7 +1435,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>51</v>
       </c>
@@ -1378,7 +1448,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
   </sheetData>
@@ -1392,22 +1462,22 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.6328125" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.08984375" customWidth="1"/>
-    <col min="5" max="5" width="57.36328125" customWidth="1"/>
-    <col min="6" max="6" width="35.453125" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="57.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1433,7 +1503,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1442,10 +1512,13 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="13"/>
+      <c r="E2" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>68</v>
       </c>
@@ -1455,16 +1528,14 @@
       <c r="C3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="D3" s="13"/>
       <c r="E3" s="13" t="s">
         <v>53</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>128</v>
       </c>
@@ -1474,16 +1545,14 @@
       <c r="C4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
         <v>132</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>134</v>
       </c>
@@ -1491,16 +1560,14 @@
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>25</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>69</v>
       </c>
@@ -1522,7 +1589,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>70</v>
       </c>
@@ -1546,7 +1613,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>71</v>
       </c>
@@ -1568,7 +1635,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>72</v>
       </c>
@@ -1590,7 +1657,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>73</v>
       </c>
@@ -1614,7 +1681,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>129</v>
       </c>
@@ -1640,7 +1707,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Update POMs to version 0.0.6. Add values to config.java Add postman environment POJ structure for processing. Update TestDataReader to consume postman environment files Update postman collection to use postman environment values. Update JAR Update sampletest to consume postman environment values.
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mposlus1\Documents\GitHub\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC95A75-B3CA-48D5-B3A8-6781609F1EEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75370450-3F1C-4C30-BC26-3E2103959B91}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26385" yWindow="2205" windowWidth="24600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="152">
   <si>
     <t>key</t>
   </si>
@@ -465,6 +465,24 @@
   </si>
   <si>
     <t>omdb.othermovies.scarymovies.Shaun.of the Dead</t>
+  </si>
+  <si>
+    <t>postman.environment.filename</t>
+  </si>
+  <si>
+    <t>PostmanEnvSample/postman_environment.json</t>
+  </si>
+  <si>
+    <t>query::apikey::{{apikey}}</t>
+  </si>
+  <si>
+    <t>query::i::{{wall-eId}}</t>
+  </si>
+  <si>
+    <t>query::i::{{lionKingId}}</t>
+  </si>
+  <si>
+    <t>query::i::{{shaunId}}</t>
   </si>
 </sst>
 </file>
@@ -876,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1192,6 +1210,14 @@
       </c>
       <c r="B33" s="11" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1462,7 +1488,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1499,7 @@
     <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="5" max="5" width="57.42578125" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1532,8 +1558,12 @@
       <c r="E3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="5"/>
+      <c r="F3" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -1549,8 +1579,12 @@
       <c r="E4" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -1564,8 +1598,12 @@
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">

</xml_diff>

<commit_message>
added sheet to sampletest that uses functions. made small change to alphanumeric generator
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mposlus1\Documents\GitHub\codeless\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75370450-3F1C-4C30-BC26-3E2103959B91}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990BD99C-6653-48A3-BEAB-1EAD98B8105F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
     <sheet name="t-googletest" sheetId="9" r:id="rId2"/>
     <sheet name="t-omdb&amp;imdb" sheetId="12" r:id="rId3"/>
+    <sheet name="t-functions" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="176">
   <si>
     <t>key</t>
   </si>
@@ -395,94 +396,166 @@
     <t>TRUE or FALSE</t>
   </si>
   <si>
+    <t>{{abc}} othervariable: {{othervar}}</t>
+  </si>
+  <si>
+    <t>74.0</t>
+  </si>
+  <si>
+    <t>waitTime::8</t>
+  </si>
+  <si>
+    <t>assertEquals::WebDriver::getTitle::{{title}}</t>
+  </si>
+  <si>
+    <t>omdb.Wall-E</t>
+  </si>
+  <si>
+    <t>omdb call2</t>
+  </si>
+  <si>
+    <t>navigate to avatar page</t>
+  </si>
+  <si>
+    <t>{{imdb2}}</t>
+  </si>
+  <si>
+    <t>omdb.othermovies.The Lion King</t>
+  </si>
+  <si>
+    <t>export::lionking_plot::JSONPATH::Plot</t>
+  </si>
+  <si>
+    <t>assertEquals::WebElement::getText::{{lionking_plot}}</t>
+  </si>
+  <si>
+    <t>omdb call3</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>test.runparallel</t>
+  </si>
+  <si>
+    <t>test.runparallel.threadcount</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>buildMode</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>qTestProjectId</t>
+  </si>
+  <si>
+    <t>qTestBuildMode</t>
+  </si>
+  <si>
+    <t>qTestTestRunId::85</t>
+  </si>
+  <si>
+    <t>omdb.othermovies.scarymovies.Shaun.of the Dead</t>
+  </si>
+  <si>
+    <t>postman.environment.filename</t>
+  </si>
+  <si>
+    <t>PostmanEnvSample/postman_environment.json</t>
+  </si>
+  <si>
+    <t>query::apikey::{{apikey}}</t>
+  </si>
+  <si>
+    <t>query::i::{{wall-eId}}</t>
+  </si>
+  <si>
+    <t>query::i::{{lionKingId}}</t>
+  </si>
+  <si>
+    <t>query::i::{{shaunId}}</t>
+  </si>
+  <si>
+    <t>type timestamp</t>
+  </si>
+  <si>
+    <t>(#timeStamp||{{format}})</t>
+  </si>
+  <si>
+    <t>type timestamp of 2 weeks ago</t>
+  </si>
+  <si>
+    <t>(#timeStamp||{{format}}||-2W)</t>
+  </si>
+  <si>
+    <t>send current timestamp</t>
+  </si>
+  <si>
+    <t>Sends a timestamp 2 weeks old</t>
+  </si>
+  <si>
+    <t>(#randNum||10)</t>
+  </si>
+  <si>
+    <t>Sends a random 10 digit number</t>
+  </si>
+  <si>
+    <t>types a random 10 digit number</t>
+  </si>
+  <si>
+    <t>types a random full name</t>
+  </si>
+  <si>
+    <t>(#randName)</t>
+  </si>
+  <si>
+    <t>Sends a random full name</t>
+  </si>
+  <si>
+    <t>types a random DOB</t>
+  </si>
+  <si>
+    <t>(#randDOB)</t>
+  </si>
+  <si>
+    <t>Sends a random date of birth</t>
+  </si>
+  <si>
+    <t>types a random alphanumeric value of length 12</t>
+  </si>
+  <si>
+    <t>(#randAlphaNum||12)</t>
+  </si>
+  <si>
+    <t>types a random alphanumeric value with format</t>
+  </si>
+  <si>
+    <t>Sends an alphanumeric value of length 12</t>
+  </si>
+  <si>
+    <t>(#randAlphaNum||DDDLLLUUUAAA)</t>
+  </si>
+  <si>
+    <t>Sends an alphanumeric value with specific format of: DDDLLLUUUAAA</t>
+  </si>
+  <si>
+    <t>types a random credit card number</t>
+  </si>
+  <si>
+    <t>(#randCCNum)</t>
+  </si>
+  <si>
+    <t>Sends a random credit card #</t>
+  </si>
+  <si>
+    <t>prod</t>
+  </si>
+  <si>
     <t>FAILUREONLY</t>
-  </si>
-  <si>
-    <t>{{abc}} othervariable: {{othervar}}</t>
-  </si>
-  <si>
-    <t>74.0</t>
-  </si>
-  <si>
-    <t>waitTime::8</t>
-  </si>
-  <si>
-    <t>assertEquals::WebDriver::getTitle::{{title}}</t>
-  </si>
-  <si>
-    <t>omdb.Wall-E</t>
-  </si>
-  <si>
-    <t>omdb call2</t>
-  </si>
-  <si>
-    <t>navigate to avatar page</t>
-  </si>
-  <si>
-    <t>{{imdb2}}</t>
-  </si>
-  <si>
-    <t>omdb.othermovies.The Lion King</t>
-  </si>
-  <si>
-    <t>export::lionking_plot::JSONPATH::Plot</t>
-  </si>
-  <si>
-    <t>assertEquals::WebElement::getText::{{lionking_plot}}</t>
-  </si>
-  <si>
-    <t>omdb call3</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>test.runparallel</t>
-  </si>
-  <si>
-    <t>test.runparallel.threadcount</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>buildMode</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>qTestProjectId</t>
-  </si>
-  <si>
-    <t>qTestBuildMode</t>
-  </si>
-  <si>
-    <t>qTestTestRunId::85</t>
-  </si>
-  <si>
-    <t>stage</t>
-  </si>
-  <si>
-    <t>omdb.othermovies.scarymovies.Shaun.of the Dead</t>
-  </si>
-  <si>
-    <t>postman.environment.filename</t>
-  </si>
-  <si>
-    <t>PostmanEnvSample/postman_environment.json</t>
-  </si>
-  <si>
-    <t>query::apikey::{{apikey}}</t>
-  </si>
-  <si>
-    <t>query::i::{{wall-eId}}</t>
-  </si>
-  <si>
-    <t>query::i::{{lionKingId}}</t>
-  </si>
-  <si>
-    <t>query::i::{{shaunId}}</t>
   </si>
 </sst>
 </file>
@@ -896,19 +969,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.42578125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.5703125" style="7"/>
+    <col min="1" max="1" width="36.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.54296875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -919,7 +992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -930,7 +1003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -941,7 +1014,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -952,7 +1025,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
@@ -963,7 +1036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -974,7 +1047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -985,18 +1058,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1007,7 +1080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>35</v>
       </c>
@@ -1018,7 +1091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
@@ -1029,7 +1102,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>38</v>
       </c>
@@ -1040,7 +1113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
@@ -1051,7 +1124,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>42</v>
       </c>
@@ -1062,49 +1135,49 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>86</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>115</v>
       </c>
@@ -1115,7 +1188,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>45</v>
       </c>
@@ -1126,18 +1199,18 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
         <v>117</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>83</v>
       </c>
@@ -1148,7 +1221,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>99</v>
       </c>
@@ -1159,12 +1232,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>102</v>
       </c>
@@ -1172,52 +1245,52 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
+      <c r="B30" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="11" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="11" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
+      <c r="B31" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="11" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="11" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>146</v>
-      </c>
       <c r="B34" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1231,23 +1304,23 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.5703125" style="1"/>
+    <col min="9" max="16384" width="8.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1346,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1284,7 +1357,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>78</v>
       </c>
@@ -1310,7 +1383,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>77</v>
       </c>
@@ -1332,7 +1405,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>80</v>
       </c>
@@ -1354,7 +1427,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>67</v>
       </c>
@@ -1370,7 +1443,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
@@ -1392,7 +1465,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>88</v>
       </c>
@@ -1406,14 +1479,14 @@
         <v>89</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
@@ -1429,7 +1502,7 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>94</v>
       </c>
@@ -1447,7 +1520,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>95</v>
       </c>
@@ -1458,10 +1531,10 @@
         <v>97</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>51</v>
       </c>
@@ -1474,7 +1547,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
   </sheetData>
@@ -1487,23 +1560,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="57.42578125" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" customWidth="1"/>
+    <col min="5" max="5" width="57.453125" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="35.54296875" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1529,7 +1602,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1539,12 +1612,12 @@
       <c r="C2" s="2"/>
       <c r="D2" s="13"/>
       <c r="E2" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>68</v>
       </c>
@@ -1552,60 +1625,60 @@
         <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13" t="s">
         <v>53</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F4" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>69</v>
       </c>
@@ -1627,7 +1700,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>70</v>
       </c>
@@ -1651,7 +1724,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>71</v>
       </c>
@@ -1673,7 +1746,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>72</v>
       </c>
@@ -1695,7 +1768,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>73</v>
       </c>
@@ -1713,15 +1786,15 @@
         <v>57</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>49</v>
@@ -1730,22 +1803,22 @@
         <v>65</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>57</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1757,4 +1830,216 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A05232-BFCE-4446-B9EB-4225BD1AF73E}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="48.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added missing fields, Refactored the code, Added e2e test
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO12\codeless_selenium_Ide_integration\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990BD99C-6653-48A3-BEAB-1EAD98B8105F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
     <sheet name="t-googletest" sheetId="9" r:id="rId2"/>
     <sheet name="t-omdb&amp;imdb" sheetId="12" r:id="rId3"/>
     <sheet name="t-functions" sheetId="13" r:id="rId4"/>
+    <sheet name="t-exceltoexcel" sheetId="14" r:id="rId5"/>
+    <sheet name="t-exceltocsv" sheetId="15" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="180">
   <si>
     <t>key</t>
   </si>
@@ -432,9 +433,6 @@
     <t>omdb call3</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>test.runparallel</t>
   </si>
   <si>
@@ -556,12 +554,27 @@
   </si>
   <si>
     <t>FAILUREONLY</t>
+  </si>
+  <si>
+    <t>execute component</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>test.soaptest</t>
+  </si>
+  <si>
+    <t>test.alpha</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -966,22 +979,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.54296875" style="7"/>
+    <col min="1" max="1" width="36.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.5546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -992,7 +1005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -1003,7 +1016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -1025,7 +1038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
@@ -1036,7 +1049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -1047,7 +1060,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -1058,7 +1071,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -1069,7 +1082,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1080,7 +1093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>35</v>
       </c>
@@ -1091,7 +1104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
@@ -1102,7 +1115,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>38</v>
       </c>
@@ -1113,7 +1126,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
@@ -1124,7 +1137,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>42</v>
       </c>
@@ -1135,49 +1148,49 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>86</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>115</v>
       </c>
@@ -1188,7 +1201,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>45</v>
       </c>
@@ -1199,18 +1212,18 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>117</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>83</v>
       </c>
@@ -1221,7 +1234,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>99</v>
       </c>
@@ -1232,12 +1245,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>102</v>
       </c>
@@ -1245,52 +1258,52 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
+      <c r="B30" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="11" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="11" t="s">
+      <c r="B31" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1300,27 +1313,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.54296875" style="1"/>
+    <col min="9" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1346,7 +1359,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1357,7 +1370,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>78</v>
       </c>
@@ -1383,7 +1396,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>77</v>
       </c>
@@ -1405,7 +1418,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>80</v>
       </c>
@@ -1427,7 +1440,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>67</v>
       </c>
@@ -1443,7 +1456,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
@@ -1465,7 +1478,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>88</v>
       </c>
@@ -1486,7 +1499,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
@@ -1502,7 +1515,7 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>94</v>
       </c>
@@ -1520,7 +1533,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>95</v>
       </c>
@@ -1534,7 +1547,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>51</v>
       </c>
@@ -1547,7 +1560,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
     </row>
   </sheetData>
@@ -1557,26 +1570,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.1796875" customWidth="1"/>
-    <col min="5" max="5" width="57.453125" customWidth="1"/>
-    <col min="6" max="6" width="35.453125" customWidth="1"/>
-    <col min="7" max="7" width="35.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="44.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.21875" customWidth="1"/>
+    <col min="5" max="5" width="57.44140625" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="35.5546875" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1615,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1612,12 +1625,12 @@
       <c r="C2" s="2"/>
       <c r="D2" s="13"/>
       <c r="E2" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>68</v>
       </c>
@@ -1632,13 +1645,13 @@
         <v>53</v>
       </c>
       <c r="F3" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>127</v>
       </c>
@@ -1653,13 +1666,13 @@
         <v>131</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>133</v>
       </c>
@@ -1667,18 +1680,18 @@
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>69</v>
       </c>
@@ -1700,7 +1713,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>70</v>
       </c>
@@ -1724,7 +1737,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>71</v>
       </c>
@@ -1746,7 +1759,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>72</v>
       </c>
@@ -1768,7 +1781,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>73</v>
       </c>
@@ -1792,7 +1805,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>128</v>
       </c>
@@ -1818,7 +1831,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1833,21 +1846,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A05232-BFCE-4446-B9EB-4225BD1AF73E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1867,7 +1880,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1878,7 +1891,7 @@
       <c r="D2" s="13"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>67</v>
       </c>
@@ -1894,9 +1907,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>27</v>
@@ -1905,16 +1918,16 @@
         <v>97</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -1923,15 +1936,15 @@
         <v>97</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>27</v>
@@ -1940,15 +1953,15 @@
         <v>97</v>
       </c>
       <c r="D6" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>27</v>
@@ -1957,15 +1970,15 @@
         <v>97</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
@@ -1974,15 +1987,15 @@
         <v>97</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
@@ -1991,15 +2004,15 @@
         <v>97</v>
       </c>
       <c r="D9" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F9" s="4" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -2008,15 +2021,15 @@
         <v>97</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -2025,19 +2038,145 @@
         <v>97</v>
       </c>
       <c r="D11" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>52</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added number and string functions modified postman environment file datareader for it to work in unit tests as well
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO12\codeless_selenium_Ide_integration\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D714A4C-28A3-4929-AF1B-DC03081BF683}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
     <sheet name="t-googletest" sheetId="9" r:id="rId2"/>
     <sheet name="t-omdb&amp;imdb" sheetId="12" r:id="rId3"/>
     <sheet name="t-functions" sheetId="13" r:id="rId4"/>
-    <sheet name="t-exceltoexcel" sheetId="14" r:id="rId5"/>
-    <sheet name="t-exceltocsv" sheetId="15" r:id="rId6"/>
+    <sheet name="t-exceltocsv" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="176">
   <si>
     <t>key</t>
   </si>
@@ -190,9 +190,6 @@
     <t>close</t>
   </si>
   <si>
-    <t>export::wall-e_plot::JSONPATH::Plot</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
@@ -256,12 +253,6 @@
     <t>path::id::{{empId}}</t>
   </si>
   <si>
-    <t>export::empId::JSONPATH::id</t>
-  </si>
-  <si>
-    <t>export::empsalary::JSONPATH::salary</t>
-  </si>
-  <si>
     <t>GET call from customer api</t>
   </si>
   <si>
@@ -343,9 +334,6 @@
     <t>com.tmobile.etp.codeless.plugin.reporting.CodelessPluginManager</t>
   </si>
   <si>
-    <t>body::string::{"name":"etptest-100","salary":"123456789","age":"100"}</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -445,15 +433,6 @@
     <t>buildMode</t>
   </si>
   <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>qTestProjectId</t>
-  </si>
-  <si>
-    <t>qTestBuildMode</t>
-  </si>
-  <si>
     <t>qTestTestRunId::85</t>
   </si>
   <si>
@@ -469,9 +448,6 @@
     <t>query::apikey::{{apikey}}</t>
   </si>
   <si>
-    <t>query::i::{{wall-eId}}</t>
-  </si>
-  <si>
     <t>query::i::{{lionKingId}}</t>
   </si>
   <si>
@@ -550,31 +526,46 @@
     <t>Sends a random credit card #</t>
   </si>
   <si>
+    <t>FAILUREONLY</t>
+  </si>
+  <si>
+    <t>execute component</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>test.alpha</t>
+  </si>
+  <si>
+    <t>export::empsalary::JSONPATH::salary
+export::empId::JSONPATH::id</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>write.test.log</t>
+  </si>
+  <si>
+    <t>leave.test.log</t>
+  </si>
+  <si>
     <t>prod</t>
   </si>
   <si>
-    <t>FAILUREONLY</t>
-  </si>
-  <si>
-    <t>execute component</t>
-  </si>
-  <si>
-    <t>component</t>
-  </si>
-  <si>
-    <t>test.soaptest</t>
-  </si>
-  <si>
-    <t>test.alpha</t>
-  </si>
-  <si>
-    <t>false</t>
+    <t>body::string::{"name":"etptest-105","salary":"123456789","age":"100"}</t>
+  </si>
+  <si>
+    <t>export::wall-e_plot::JSONPATH::Plot
+query::apikey::{{apikey}}
+query::i::{{wall-eId}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -667,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -698,6 +689,9 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -979,22 +973,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.5546875" style="7"/>
+    <col min="1" max="1" width="36.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.54296875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -1016,7 +1010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -1027,7 +1021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -1038,7 +1032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
@@ -1049,7 +1043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -1060,7 +1054,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
@@ -1071,18 +1065,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1093,7 +1087,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>35</v>
       </c>
@@ -1104,7 +1098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
@@ -1115,7 +1109,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>38</v>
       </c>
@@ -1126,7 +1120,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
@@ -1137,7 +1131,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>42</v>
       </c>
@@ -1148,60 +1142,60 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>87</v>
-      </c>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>45</v>
       </c>
@@ -1209,101 +1203,101 @@
         <v>26</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1313,27 +1307,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B12"/>
+    <sheetView topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.5546875" style="1"/>
+    <col min="9" max="16384" width="8.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1356,10 +1350,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1370,9 +1364,9 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
@@ -1384,21 +1378,19 @@
         <v>47</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>75</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="6"/>
       <c r="H3" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>18</v>
@@ -1410,39 +1402,39 @@
         <v>25</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>49</v>
@@ -1453,101 +1445,101 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>51</v>
       </c>
@@ -1557,10 +1549,10 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="H12" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
   </sheetData>
@@ -1570,26 +1562,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="44.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.21875" customWidth="1"/>
-    <col min="5" max="5" width="57.44140625" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
-    <col min="7" max="7" width="35.5546875" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" customWidth="1"/>
+    <col min="5" max="5" width="57.453125" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="35.54296875" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1612,10 +1604,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1625,213 +1617,209 @@
       <c r="C2" s="2"/>
       <c r="D2" s="13"/>
       <c r="E2" s="12" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D3" s="13"/>
-      <c r="E3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="F7" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="G10" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>128</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1846,21 +1834,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1877,10 +1865,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1891,9 +1879,9 @@
       <c r="D2" s="13"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>49</v>
@@ -1904,147 +1892,147 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
         <v>162</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>170</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>51</v>
       </c>
@@ -2058,23 +2046,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2091,7 +2079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -2102,78 +2090,15 @@
       <c r="D2" s="13"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="12"/>

</xml_diff>

<commit_message>
updated poms checked in new jar
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D714A4C-28A3-4929-AF1B-DC03081BF683}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7714F4F1-F028-40DA-AD73-861F3F340D48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="180">
   <si>
     <t>key</t>
   </si>
@@ -560,6 +560,19 @@
     <t>export::wall-e_plot::JSONPATH::Plot
 query::apikey::{{apikey}}
 query::i::{{wall-eId}}</t>
+  </si>
+  <si>
+    <t>does an addition function</t>
+  </si>
+  <si>
+    <t>(#Math||add||25||3.5)</t>
+  </si>
+  <si>
+    <t>path::id::{{empId}}
+header::sumtest::(#Math||add||5||{{empsalary}})</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -976,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1297,7 +1310,7 @@
         <v>172</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1311,7 +1324,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1388,7 +1401,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>74</v>
       </c>
@@ -1401,8 +1414,8 @@
       <c r="D4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>73</v>
+      <c r="E4" s="17" t="s">
+        <v>178</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
@@ -1565,7 +1578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1835,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2032,11 +2045,32 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="13"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B14" s="13" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated google model. uploaded new sampletest with more function tests
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7714F4F1-F028-40DA-AD73-861F3F340D48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D2E551-A1C8-44D8-A8EA-C2D38B76441D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="186">
   <si>
     <t>key</t>
   </si>
@@ -299,9 +299,6 @@
   </si>
   <si>
     <t>move</t>
-  </si>
-  <si>
-    <t>export::abc::WebElement::getText</t>
   </si>
   <si>
     <t>get text of the element</t>
@@ -573,6 +570,28 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>does a mod function</t>
+  </si>
+  <si>
+    <t>(#Math||mod||108||10)</t>
+  </si>
+  <si>
+    <t>does the string function uppercase</t>
+  </si>
+  <si>
+    <t>does the string function substring</t>
+  </si>
+  <si>
+    <t>(#String||substring||this is my a sentence||13||20)</t>
+  </si>
+  <si>
+    <t>(#String||upperCase||mystring)</t>
+  </si>
+  <si>
+    <t>waitType::visible
+export::abc::WebElement::getText</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1083,7 +1102,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>33</v>
@@ -1199,13 +1218,13 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
@@ -1216,18 +1235,18 @@
         <v>26</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -1235,82 +1254,82 @@
         <v>80</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1323,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1363,7 +1382,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1391,14 +1410,14 @@
         <v>47</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -1415,12 +1434,12 @@
         <v>25</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1442,7 +1461,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1458,7 +1477,7 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1469,7 +1488,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>88</v>
@@ -1480,7 +1499,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1491,17 +1510,17 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>86</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1512,7 +1531,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
@@ -1520,36 +1539,34 @@
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>90</v>
-      </c>
+      <c r="E10" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1562,7 +1579,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="H12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1617,7 +1634,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1630,7 +1647,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="13"/>
       <c r="E2" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
@@ -1643,53 +1660,53 @@
         <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1707,11 +1724,11 @@
         <v>56</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1731,11 +1748,11 @@
         <v>59</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1753,11 +1770,11 @@
         <v>62</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1775,11 +1792,11 @@
         <v>62</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1800,15 +1817,15 @@
         <v>56</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>49</v>
@@ -1817,19 +1834,19 @@
         <v>64</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>56</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1848,10 +1865,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1878,7 +1895,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1905,172 +1922,211 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>160</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="13"/>
+      <c r="A13" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>180</v>
+      </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B16" s="13" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2126,13 +2182,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="12"/>

</xml_diff>

<commit_message>
update web drivers and fix the copy issue
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C94139\Desktop\myrepos\codeless\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jung\Documents\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D2E551-A1C8-44D8-A8EA-C2D38B76441D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546A3243-2E3D-4DAA-9914-F97CF80CA9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>web_drivers/windows/chromedriver.exe</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>serviceCall</t>
   </si>
   <si>
@@ -97,12 +94,6 @@
     <t>Path to the firefox webdriver to use for this machine. Installed under &lt;INSTALL_DIR&gt;/webdrivers/&lt;OS&gt; by default. For Windows: web_drivers/windows/geckodriver.exe For Mac: web_drivers/mac/geckodriver</t>
   </si>
   <si>
-    <t>webdriver.path.ie</t>
-  </si>
-  <si>
-    <t>web_drivers/windows/IEDriverServer.exe</t>
-  </si>
-  <si>
     <t>Path to the ie webdriver to use for this machine. Installed under &lt;INSTALL_DIR&gt;/webdrivers/&lt;OS&gt; by default. Windows only, no other valid settings.</t>
   </si>
   <si>
@@ -118,48 +109,18 @@
     <t>click</t>
   </si>
   <si>
-    <t>webdriver.platform.chrome</t>
-  </si>
-  <si>
     <t>Windows</t>
   </si>
   <si>
     <t>Plateform type for remote web driver intializing</t>
   </si>
   <si>
-    <t>webdriver.version.chrome</t>
-  </si>
-  <si>
     <t>Version for plateform type selected</t>
   </si>
   <si>
-    <t>webdriver.platform.ie</t>
-  </si>
-  <si>
-    <t>webdriver.version.ie</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>webdriver.platform.firefox</t>
-  </si>
-  <si>
-    <t>webdriver.version.firefox</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>webdriver.platform.safari</t>
-  </si>
-  <si>
     <t>macos 10.12</t>
   </si>
   <si>
-    <t>webdriver.version.safari</t>
-  </si>
-  <si>
     <t>9.0</t>
   </si>
   <si>
@@ -383,9 +344,6 @@
   </si>
   <si>
     <t>{{abc}} othervariable: {{othervar}}</t>
-  </si>
-  <si>
-    <t>74.0</t>
   </si>
   <si>
     <t>waitTime::8</t>
@@ -592,6 +550,48 @@
   <si>
     <t>waitType::visible
 export::abc::WebElement::getText</t>
+  </si>
+  <si>
+    <t>webdriver.platformName.chrome</t>
+  </si>
+  <si>
+    <t>webdriver.browserVersion.chrome</t>
+  </si>
+  <si>
+    <t>webdriver.platformName.firefox</t>
+  </si>
+  <si>
+    <t>webdriver.platformName.safari</t>
+  </si>
+  <si>
+    <t>webdriver.browserVersion.firefox</t>
+  </si>
+  <si>
+    <t>webdriver.browserVersion.safari</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>91.0</t>
+  </si>
+  <si>
+    <t>webdriver.path.edge</t>
+  </si>
+  <si>
+    <t>web_drivers/windows/msedgedriver.exe</t>
+  </si>
+  <si>
+    <t>webdriver.platformName.edge</t>
+  </si>
+  <si>
+    <t>webdriver.browserVersion.edge</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -1008,19 +1008,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.453125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.54296875" style="7"/>
+    <col min="1" max="1" width="36.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1031,29 +1031,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -1064,272 +1064,272 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="11" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="C22" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="37" x14ac:dyDescent="0.45">
-      <c r="A23" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="37" x14ac:dyDescent="0.45">
-      <c r="A24" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="B31" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1342,24 +1342,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.54296875" style="1"/>
+    <col min="9" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1382,10 +1382,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1396,193 +1396,193 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="13" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>120</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="17" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="H12" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
   </sheetData>
@@ -1599,19 +1599,19 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="44.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.1796875" customWidth="1"/>
-    <col min="5" max="5" width="57.453125" customWidth="1"/>
-    <col min="6" max="6" width="35.453125" customWidth="1"/>
-    <col min="7" max="7" width="35.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="57.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
     <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1634,10 +1634,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1647,214 +1647,214 @@
       <c r="C2" s="2"/>
       <c r="D2" s="13"/>
       <c r="E2" s="12" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="17" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="13" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="12" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="H10" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="B11" s="13" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1871,14 +1871,14 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1895,10 +1895,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1909,225 +1909,225 @@
       <c r="D2" s="13"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="13" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="13" t="s">
+    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="B7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>159</v>
-      </c>
       <c r="F7" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="F11" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+    </row>
+    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>176</v>
-      </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2143,16 +2143,16 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -2180,15 +2180,15 @@
       <c r="D2" s="13"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="12"/>

</xml_diff>

<commit_message>
Upgrade to use Selenium 4
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampletest.xlsx
+++ b/example_usage/suites/sampletest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jung\Documents\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546A3243-2E3D-4DAA-9914-F97CF80CA9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A918DD5-69FA-4479-8404-28EFF915D23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -591,7 +591,7 @@
     <t>91</t>
   </si>
   <si>
-    <t>firefox</t>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>